<commit_message>
update ratings table filledin
</commit_message>
<xml_diff>
--- a/Examples/AHP_Ratings_Employee_Evaluation/Ratings_Employee_Eval_ratingsresults.xlsx
+++ b/Examples/AHP_Ratings_Employee_Evaluation/Ratings_Employee_Eval_ratingsresults.xlsx
@@ -42,7 +42,7 @@
       <color rgb="ff000000"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="13">
     <fill>
       <patternFill/>
     </fill>
@@ -95,11 +95,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="00f9d5b6"/>
         <bgColor rgb="00f9d5b6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="ffcde4f7"/>
       </patternFill>
     </fill>
     <fill>
@@ -168,9 +163,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="3" fillId="11" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="12" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="3" fillId="10" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="11" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -2122,7 +2117,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2406,287 +2401,287 @@
       <c r="J9" s="17" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="B11" s="15" t="inlineStr">
+      <c r="B11" s="7" t="n">
+        <v>0.07727187447510635</v>
+      </c>
+      <c r="C11" s="7" t="n">
+        <v>0.1925982192678802</v>
+      </c>
+      <c r="D11" s="7" t="n">
+        <v>0.04879821520584188</v>
+      </c>
+      <c r="E11" s="7" t="n">
+        <v>0.3626604749641593</v>
+      </c>
+      <c r="F11" s="7" t="n">
+        <v>0.2353880186521438</v>
+      </c>
+      <c r="G11" s="7" t="n">
+        <v>0.05080275595694478</v>
+      </c>
+      <c r="H11" s="7" t="n">
+        <v>0.03248044147792362</v>
+      </c>
+      <c r="I11" s="18" t="inlineStr">
+        <is>
+          <t>TOTALS</t>
+        </is>
+      </c>
+      <c r="J11" s="18" t="inlineStr">
+        <is>
+          <t>PRIORITIES</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="15" t="inlineStr">
         <is>
           <t>Dependability</t>
         </is>
       </c>
-      <c r="C11" s="15" t="inlineStr">
+      <c r="C12" s="15" t="inlineStr">
         <is>
           <t>Education</t>
         </is>
       </c>
-      <c r="D11" s="15" t="inlineStr">
+      <c r="D12" s="15" t="inlineStr">
         <is>
           <t>Experience</t>
         </is>
       </c>
-      <c r="E11" s="15" t="inlineStr">
+      <c r="E12" s="15" t="inlineStr">
         <is>
           <t>Attitude</t>
         </is>
       </c>
-      <c r="F11" s="15" t="inlineStr">
+      <c r="F12" s="15" t="inlineStr">
         <is>
           <t>Leadership</t>
         </is>
       </c>
-      <c r="G11" s="15" t="inlineStr">
+      <c r="G12" s="15" t="inlineStr">
         <is>
           <t>Quantity</t>
         </is>
       </c>
-      <c r="H11" s="15" t="inlineStr">
+      <c r="H12" s="15" t="inlineStr">
         <is>
           <t>Quality</t>
         </is>
       </c>
-      <c r="I11" s="18" t="inlineStr">
-        <is>
-          <t>TOTALS</t>
-        </is>
-      </c>
-      <c r="J11" s="18" t="inlineStr">
-        <is>
-          <t>PRIORITIES</t>
-        </is>
-      </c>
     </row>
     <row r="13">
-      <c r="B13" s="7" t="n">
-        <v>0.07727187447510635</v>
-      </c>
-      <c r="C13" s="7" t="n">
-        <v>0.1925982192678802</v>
-      </c>
-      <c r="D13" s="7" t="n">
-        <v>0.04879821520584188</v>
-      </c>
-      <c r="E13" s="7" t="n">
-        <v>0.3626604749641593</v>
-      </c>
-      <c r="F13" s="7" t="n">
-        <v>0.2353880186521438</v>
-      </c>
-      <c r="G13" s="7" t="n">
-        <v>0.05080275595694478</v>
-      </c>
-      <c r="H13" s="7" t="n">
-        <v>0.03248044147792362</v>
+      <c r="A13" s="15" t="inlineStr">
+        <is>
+          <t>Jim Kendall</t>
+        </is>
+      </c>
+      <c r="B13" s="7">
+        <f>INDEX(rating_scales!J3:J7, MATCH(B2,rating_scales!A3:A7, 0))</f>
+        <v/>
+      </c>
+      <c r="C13" s="7">
+        <f>INDEX(rating_scales!I13:I16, MATCH(C2,rating_scales!A13:A16, 0))</f>
+        <v/>
+      </c>
+      <c r="D13" s="7">
+        <f>INDEX(rating_scales!I22:I25, MATCH(D2,rating_scales!A22:A25, 0))</f>
+        <v/>
+      </c>
+      <c r="E13" s="7">
+        <f>INDEX(rating_scales!I31:I34, MATCH(E2,rating_scales!A31:A34, 0))</f>
+        <v/>
+      </c>
+      <c r="F13" s="7">
+        <f>INDEX(rating_scales!J40:J44, MATCH(F2,rating_scales!A40:A44, 0))</f>
+        <v/>
+      </c>
+      <c r="G13" s="7">
+        <f>INDEX(rating_scales!I50:I53, MATCH(G2,rating_scales!A50:A53, 0))</f>
+        <v/>
+      </c>
+      <c r="H13" s="7">
+        <f>INDEX(rating_scales!I59:I62, MATCH(H2,rating_scales!A59:A62, 0))</f>
+        <v/>
+      </c>
+      <c r="I13" s="19">
+        <f>sumproduct(B13:H13,B11:H11)</f>
+        <v/>
+      </c>
+      <c r="J13" s="20">
+        <f>I13/sum(I13:I17)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="15" t="inlineStr">
+        <is>
+          <t>Sally Brown</t>
+        </is>
+      </c>
+      <c r="B14" s="7">
+        <f>INDEX(rating_scales!J3:J7, MATCH(B3,rating_scales!A3:A7, 0))</f>
+        <v/>
+      </c>
+      <c r="C14" s="7">
+        <f>INDEX(rating_scales!I13:I16, MATCH(C3,rating_scales!A13:A16, 0))</f>
+        <v/>
+      </c>
+      <c r="D14" s="7">
+        <f>INDEX(rating_scales!I22:I25, MATCH(D3,rating_scales!A22:A25, 0))</f>
+        <v/>
+      </c>
+      <c r="E14" s="7">
+        <f>INDEX(rating_scales!I31:I34, MATCH(E3,rating_scales!A31:A34, 0))</f>
+        <v/>
+      </c>
+      <c r="F14" s="7">
+        <f>INDEX(rating_scales!J40:J44, MATCH(F3,rating_scales!A40:A44, 0))</f>
+        <v/>
+      </c>
+      <c r="G14" s="7">
+        <f>INDEX(rating_scales!I50:I53, MATCH(G3,rating_scales!A50:A53, 0))</f>
+        <v/>
+      </c>
+      <c r="H14" s="7">
+        <f>INDEX(rating_scales!I59:I62, MATCH(H3,rating_scales!A59:A62, 0))</f>
+        <v/>
+      </c>
+      <c r="I14" s="19">
+        <f>sumproduct(B14:H14,B11:H11)</f>
+        <v/>
+      </c>
+      <c r="J14" s="20">
+        <f>I14/sum(I13:I17)</f>
+        <v/>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="15" t="inlineStr">
         <is>
-          <t>Jim Kendall</t>
+          <t>John Carter</t>
         </is>
       </c>
       <c r="B15" s="7">
-        <f>INDEX(rating_scales!J3:J7, MATCH(B2,rating_scales!A3:A7, 0))</f>
+        <f>INDEX(rating_scales!J3:J7, MATCH(B4,rating_scales!A3:A7, 0))</f>
         <v/>
       </c>
       <c r="C15" s="7">
-        <f>INDEX(rating_scales!I13:I16, MATCH(C2,rating_scales!A13:A16, 0))</f>
+        <f>INDEX(rating_scales!I13:I16, MATCH(C4,rating_scales!A13:A16, 0))</f>
         <v/>
       </c>
       <c r="D15" s="7">
-        <f>INDEX(rating_scales!I22:I25, MATCH(D2,rating_scales!A22:A25, 0))</f>
+        <f>INDEX(rating_scales!I22:I25, MATCH(D4,rating_scales!A22:A25, 0))</f>
         <v/>
       </c>
       <c r="E15" s="7">
-        <f>INDEX(rating_scales!I31:I34, MATCH(E2,rating_scales!A31:A34, 0))</f>
+        <f>INDEX(rating_scales!I31:I34, MATCH(E4,rating_scales!A31:A34, 0))</f>
         <v/>
       </c>
       <c r="F15" s="7">
-        <f>INDEX(rating_scales!J40:J44, MATCH(F2,rating_scales!A40:A44, 0))</f>
+        <f>INDEX(rating_scales!J40:J44, MATCH(F4,rating_scales!A40:A44, 0))</f>
         <v/>
       </c>
       <c r="G15" s="7">
-        <f>INDEX(rating_scales!I50:I53, MATCH(G2,rating_scales!A50:A53, 0))</f>
+        <f>INDEX(rating_scales!I50:I53, MATCH(G4,rating_scales!A50:A53, 0))</f>
         <v/>
       </c>
       <c r="H15" s="7">
-        <f>INDEX(rating_scales!I59:I62, MATCH(H2,rating_scales!A59:A62, 0))</f>
+        <f>INDEX(rating_scales!I59:I62, MATCH(H4,rating_scales!A59:A62, 0))</f>
         <v/>
       </c>
       <c r="I15" s="19">
-        <f>sumproduct(B15:H15,B13:H13)</f>
+        <f>sumproduct(B15:H15,B11:H11)</f>
         <v/>
       </c>
       <c r="J15" s="20">
-        <f>I15/sum(I15:I19)</f>
+        <f>I15/sum(I13:I17)</f>
         <v/>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="15" t="inlineStr">
         <is>
-          <t>Sally Brown</t>
+          <t>Mi Sung</t>
         </is>
       </c>
       <c r="B16" s="7">
-        <f>INDEX(rating_scales!J3:J7, MATCH(B3,rating_scales!A3:A7, 0))</f>
+        <f>INDEX(rating_scales!J3:J7, MATCH(B5,rating_scales!A3:A7, 0))</f>
         <v/>
       </c>
       <c r="C16" s="7">
-        <f>INDEX(rating_scales!I13:I16, MATCH(C3,rating_scales!A13:A16, 0))</f>
+        <f>INDEX(rating_scales!I13:I16, MATCH(C5,rating_scales!A13:A16, 0))</f>
         <v/>
       </c>
       <c r="D16" s="7">
-        <f>INDEX(rating_scales!I22:I25, MATCH(D3,rating_scales!A22:A25, 0))</f>
+        <f>INDEX(rating_scales!I22:I25, MATCH(D5,rating_scales!A22:A25, 0))</f>
         <v/>
       </c>
       <c r="E16" s="7">
-        <f>INDEX(rating_scales!I31:I34, MATCH(E3,rating_scales!A31:A34, 0))</f>
+        <f>INDEX(rating_scales!I31:I34, MATCH(E5,rating_scales!A31:A34, 0))</f>
         <v/>
       </c>
       <c r="F16" s="7">
-        <f>INDEX(rating_scales!J40:J44, MATCH(F3,rating_scales!A40:A44, 0))</f>
+        <f>INDEX(rating_scales!J40:J44, MATCH(F5,rating_scales!A40:A44, 0))</f>
         <v/>
       </c>
       <c r="G16" s="7">
-        <f>INDEX(rating_scales!I50:I53, MATCH(G3,rating_scales!A50:A53, 0))</f>
+        <f>INDEX(rating_scales!I50:I53, MATCH(G5,rating_scales!A50:A53, 0))</f>
         <v/>
       </c>
       <c r="H16" s="7">
-        <f>INDEX(rating_scales!I59:I62, MATCH(H3,rating_scales!A59:A62, 0))</f>
+        <f>INDEX(rating_scales!I59:I62, MATCH(H5,rating_scales!A59:A62, 0))</f>
         <v/>
       </c>
       <c r="I16" s="19">
-        <f>sumproduct(B16:H16,B13:H13)</f>
+        <f>sumproduct(B16:H16,B11:H11)</f>
         <v/>
       </c>
       <c r="J16" s="20">
-        <f>I16/sum(I15:I19)</f>
+        <f>I16/sum(I13:I17)</f>
         <v/>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="15" t="inlineStr">
         <is>
-          <t>John Carter</t>
+          <t>Arturo Chavez</t>
         </is>
       </c>
       <c r="B17" s="7">
-        <f>INDEX(rating_scales!J3:J7, MATCH(B4,rating_scales!A3:A7, 0))</f>
+        <f>INDEX(rating_scales!J3:J7, MATCH(B6,rating_scales!A3:A7, 0))</f>
         <v/>
       </c>
       <c r="C17" s="7">
-        <f>INDEX(rating_scales!I13:I16, MATCH(C4,rating_scales!A13:A16, 0))</f>
+        <f>INDEX(rating_scales!I13:I16, MATCH(C6,rating_scales!A13:A16, 0))</f>
         <v/>
       </c>
       <c r="D17" s="7">
-        <f>INDEX(rating_scales!I22:I25, MATCH(D4,rating_scales!A22:A25, 0))</f>
+        <f>INDEX(rating_scales!I22:I25, MATCH(D6,rating_scales!A22:A25, 0))</f>
         <v/>
       </c>
       <c r="E17" s="7">
-        <f>INDEX(rating_scales!I31:I34, MATCH(E4,rating_scales!A31:A34, 0))</f>
+        <f>INDEX(rating_scales!I31:I34, MATCH(E6,rating_scales!A31:A34, 0))</f>
         <v/>
       </c>
       <c r="F17" s="7">
-        <f>INDEX(rating_scales!J40:J44, MATCH(F4,rating_scales!A40:A44, 0))</f>
+        <f>INDEX(rating_scales!J40:J44, MATCH(F6,rating_scales!A40:A44, 0))</f>
         <v/>
       </c>
       <c r="G17" s="7">
-        <f>INDEX(rating_scales!I50:I53, MATCH(G4,rating_scales!A50:A53, 0))</f>
+        <f>INDEX(rating_scales!I50:I53, MATCH(G6,rating_scales!A50:A53, 0))</f>
         <v/>
       </c>
       <c r="H17" s="7">
-        <f>INDEX(rating_scales!I59:I62, MATCH(H4,rating_scales!A59:A62, 0))</f>
+        <f>INDEX(rating_scales!I59:I62, MATCH(H6,rating_scales!A59:A62, 0))</f>
         <v/>
       </c>
       <c r="I17" s="19">
-        <f>sumproduct(B17:H17,B13:H13)</f>
+        <f>sumproduct(B17:H17,B11:H11)</f>
         <v/>
       </c>
       <c r="J17" s="20">
-        <f>I17/sum(I15:I19)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="15" t="inlineStr">
-        <is>
-          <t>Mi Sung</t>
-        </is>
-      </c>
-      <c r="B18" s="7">
-        <f>INDEX(rating_scales!J3:J7, MATCH(B5,rating_scales!A3:A7, 0))</f>
-        <v/>
-      </c>
-      <c r="C18" s="7">
-        <f>INDEX(rating_scales!I13:I16, MATCH(C5,rating_scales!A13:A16, 0))</f>
-        <v/>
-      </c>
-      <c r="D18" s="7">
-        <f>INDEX(rating_scales!I22:I25, MATCH(D5,rating_scales!A22:A25, 0))</f>
-        <v/>
-      </c>
-      <c r="E18" s="7">
-        <f>INDEX(rating_scales!I31:I34, MATCH(E5,rating_scales!A31:A34, 0))</f>
-        <v/>
-      </c>
-      <c r="F18" s="7">
-        <f>INDEX(rating_scales!J40:J44, MATCH(F5,rating_scales!A40:A44, 0))</f>
-        <v/>
-      </c>
-      <c r="G18" s="7">
-        <f>INDEX(rating_scales!I50:I53, MATCH(G5,rating_scales!A50:A53, 0))</f>
-        <v/>
-      </c>
-      <c r="H18" s="7">
-        <f>INDEX(rating_scales!I59:I62, MATCH(H5,rating_scales!A59:A62, 0))</f>
-        <v/>
-      </c>
-      <c r="I18" s="19">
-        <f>sumproduct(B18:H18,B13:H13)</f>
-        <v/>
-      </c>
-      <c r="J18" s="20">
-        <f>I18/sum(I15:I19)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="15" t="inlineStr">
-        <is>
-          <t>Arturo Chavez</t>
-        </is>
-      </c>
-      <c r="B19" s="7">
-        <f>INDEX(rating_scales!J3:J7, MATCH(B6,rating_scales!A3:A7, 0))</f>
-        <v/>
-      </c>
-      <c r="C19" s="7">
-        <f>INDEX(rating_scales!I13:I16, MATCH(C6,rating_scales!A13:A16, 0))</f>
-        <v/>
-      </c>
-      <c r="D19" s="7">
-        <f>INDEX(rating_scales!I22:I25, MATCH(D6,rating_scales!A22:A25, 0))</f>
-        <v/>
-      </c>
-      <c r="E19" s="7">
-        <f>INDEX(rating_scales!I31:I34, MATCH(E6,rating_scales!A31:A34, 0))</f>
-        <v/>
-      </c>
-      <c r="F19" s="7">
-        <f>INDEX(rating_scales!J40:J44, MATCH(F6,rating_scales!A40:A44, 0))</f>
-        <v/>
-      </c>
-      <c r="G19" s="7">
-        <f>INDEX(rating_scales!I50:I53, MATCH(G6,rating_scales!A50:A53, 0))</f>
-        <v/>
-      </c>
-      <c r="H19" s="7">
-        <f>INDEX(rating_scales!I59:I62, MATCH(H6,rating_scales!A59:A62, 0))</f>
-        <v/>
-      </c>
-      <c r="I19" s="19">
-        <f>sumproduct(B19:H19,B13:H13)</f>
-        <v/>
-      </c>
-      <c r="J19" s="20">
-        <f>I19/sum(I15:I19)</f>
+        <f>I17/sum(I13:I17)</f>
         <v/>
       </c>
     </row>

</xml_diff>